<commit_message>
Edits to scenarios and budgets spreadsheet
</commit_message>
<xml_diff>
--- a/Scenario_details_budgets.xlsx
+++ b/Scenario_details_budgets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5D1D2-3201-44D2-8687-4989DF1C94D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C219C49-4A73-44CC-A904-31EA6FEB746D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1212E98E-316A-4462-9DDD-C4D6B4A104FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Manager budget remains constant, user budget increases</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>Test scenario</t>
   </si>
   <si>
@@ -145,6 +142,15 @@
   </si>
   <si>
     <t>Performs less well than above</t>
+  </si>
+  <si>
+    <t>T1a</t>
+  </si>
+  <si>
+    <t>T1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As above, but the amplitude is half and the period is double </t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -543,6 +549,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,6 +568,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -564,21 +585,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2889,10 +2899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9FB661-68A1-4497-AF3A-764ADECA08FB}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2909,33 +2919,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="37" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="2" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2951,10 +2961,10 @@
       <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="40"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -2982,11 +2992,11 @@
       <c r="H3" s="9">
         <v>0</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="24">
         <f>G3*50</f>
         <v>50000</v>
       </c>
-      <c r="J3" s="38"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
@@ -3014,10 +3024,10 @@
       <c r="H4" s="16">
         <v>-3</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="25">
         <v>6325</v>
       </c>
-      <c r="J4" s="38"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
@@ -3044,11 +3054,11 @@
       <c r="H5" s="9">
         <v>0</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="24">
         <f>G5*50</f>
         <v>50000</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
@@ -3065,8 +3075,8 @@
       <c r="F6" s="15"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="38"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
@@ -3083,8 +3093,8 @@
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -3112,78 +3122,96 @@
       <c r="H8" s="10">
         <v>15</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="28">
         <v>68375</v>
       </c>
-      <c r="J8" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="38" t="s">
+      <c r="I9" s="25"/>
+      <c r="J9" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+    <row r="12" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="31"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="38"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J12" s="39"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3201,512 +3229,812 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE971661-927D-4F43-BD83-FF2E27F4DD24}">
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>350</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>400</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>450</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>550</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>600</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>650</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>700</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>750</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>800</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>850</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>900</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>950</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1050</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1100</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1150</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1200</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1250</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1300</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1350</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1400</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1450</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1500</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1550</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1600</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1650</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1700</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1750</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1800</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1850</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1900</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1950</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2000</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2050</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2100</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2150</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2200</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2250</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2300</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2350</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2400</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2450</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2500</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2550</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2600</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2650</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2700</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2750</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2800</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2850</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2900</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2950</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3000</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3050</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3100</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3150</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3200</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3250</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3300</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3350</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3400</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3450</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3500</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3550</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3600</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3650</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3700</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3750</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3800</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>3850</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>3900</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>3950</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4000</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4050</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4100</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4150</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4200</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4250</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4300</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4350</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4400</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4450</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4500</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4550</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4600</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4650</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4700</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <v>9400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4750</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4800</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4850</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4900</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4950</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>5000</v>
+      </c>
+      <c r="C100">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated scenarios and budgets
</commit_message>
<xml_diff>
--- a/Scenario_details_budgets.xlsx
+++ b/Scenario_details_budgets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C219C49-4A73-44CC-A904-31EA6FEB746D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EE7277-3F47-4628-AB17-DF9D81DF3D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1212E98E-316A-4462-9DDD-C4D6B4A104FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Manager budget increases and decreases in a predictable/regular way above and below a mean (like a sine wave), user budget increases linearly</t>
   </si>
   <si>
-    <t>Manager budget increases and decreases unpredictably (drawing from Poisson distribution), user budget increases linearly</t>
-  </si>
-  <si>
     <t>I think all of these scenarios need to have the same cumulative total for the manager budget. So we are asking: given the same total budget over 50 years, what is the best way to receive/invest it?</t>
   </si>
   <si>
@@ -152,6 +149,21 @@
   <si>
     <t xml:space="preserve">As above, but the amplitude is half and the period is double </t>
   </si>
+  <si>
+    <t>Manager budget increases and decreases unpredictably (using Fourier series to create random complex waves), user budget increases linearly</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Supporting Info</t>
+  </si>
+  <si>
+    <t>Main text</t>
+  </si>
+  <si>
+    <t>Not sure I want to include the above orange scenario</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +196,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -532,11 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -561,6 +581,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,10 +615,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2899,74 +2933,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9FB661-68A1-4497-AF3A-764ADECA08FB}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="30"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2974,62 +3013,68 @@
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="9">
         <v>1000</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="9">
         <v>0</v>
       </c>
-      <c r="F3" s="8">
-        <f>D3*50</f>
+      <c r="G3" s="8">
+        <f>E3*50</f>
         <v>50000</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="9">
         <v>1000</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="9">
         <v>0</v>
       </c>
-      <c r="I3" s="24">
-        <f>G3*50</f>
+      <c r="J3" s="22">
+        <f>H3*50</f>
         <v>50000</v>
       </c>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="16">
+      <c r="E4" s="14">
         <v>1000</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F4" s="14">
         <v>0</v>
       </c>
-      <c r="F4" s="15">
-        <f>D4*50</f>
+      <c r="G4" s="13">
+        <f>E4*50</f>
         <v>50000</v>
       </c>
-      <c r="G4" s="16">
+      <c r="H4" s="14">
         <v>1000</v>
       </c>
-      <c r="H4" s="16">
+      <c r="I4" s="14">
         <v>-3</v>
       </c>
-      <c r="I4" s="25">
+      <c r="J4" s="23">
         <v>6325</v>
       </c>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -3037,189 +3082,216 @@
         <v>15</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9">
+      <c r="E5" s="9">
         <v>1000</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="9">
         <v>-3</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G5" s="8">
         <v>6325</v>
       </c>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>1000</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <v>0</v>
       </c>
-      <c r="I5" s="24">
-        <f>G5*50</f>
+      <c r="J5" s="22">
+        <f>H5*50</f>
         <v>50000</v>
       </c>
-      <c r="J5" s="30"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="30"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="30"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="3"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10">
+      <c r="E8" s="10">
         <v>1000</v>
       </c>
-      <c r="E8" s="10">
+      <c r="F8" s="10">
         <v>0</v>
       </c>
-      <c r="F8" s="11">
-        <f>D8*50</f>
+      <c r="G8" s="11">
+        <f>E8*50</f>
         <v>50000</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <v>1000</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <v>15</v>
       </c>
-      <c r="I8" s="28">
+      <c r="J8" s="26">
         <v>68375</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="K8" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+    <row r="10" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="30" t="s">
+      <c r="C10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="18" t="s">
+    <row r="12" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J13" s="31"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="5"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final scenario details spredsheet
</commit_message>
<xml_diff>
--- a/Scenario_details_budgets.xlsx
+++ b/Scenario_details_budgets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389724C6-60BC-4650-BEFD-5D6C2056DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3D5AA4-A6CC-459B-893E-4B2A1F785064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1212E98E-316A-4462-9DDD-C4D6B4A104FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -99,19 +99,7 @@
     <t>Manager budget remains constant, user budget increases</t>
   </si>
   <si>
-    <t>Test scenario</t>
-  </si>
-  <si>
-    <t>Manager budget increases in steps, user budget increases linearly</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
     <t>Manager budget increases and decreases in a predictable/regular way above and below a mean (like a sine wave), user budget increases linearly</t>
-  </si>
-  <si>
-    <t>I think all of these scenarios need to have the same cumulative total for the manager budget. So we are asking: given the same total budget over 50 years, what is the best way to receive/invest it?</t>
   </si>
   <si>
     <t>MANAGER BUDGET</t>
@@ -132,12 +120,6 @@
     <t>Performs less well than above</t>
   </si>
   <si>
-    <t xml:space="preserve">As above, but the amplitude is half and the period is double </t>
-  </si>
-  <si>
-    <t>Manager budget increases and decreases unpredictably (using Fourier series to create random complex waves), user budget increases linearly</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -145,15 +127,6 @@
   </si>
   <si>
     <t>Main text</t>
-  </si>
-  <si>
-    <t>Not sure I want to include the above orange scenario</t>
-  </si>
-  <si>
-    <t>manager budget not more than 130% of user budget</t>
-  </si>
-  <si>
-    <t>manager budget no less than 80% of user budget</t>
   </si>
   <si>
     <t>NA</t>
@@ -166,6 +139,33 @@
   </si>
   <si>
     <t>~2-3 years</t>
+  </si>
+  <si>
+    <t>manager budget not more than 140% of user budget</t>
+  </si>
+  <si>
+    <t>manager budget no less than 70% of user budget</t>
+  </si>
+  <si>
+    <t>Sine wave</t>
+  </si>
+  <si>
+    <t>Random complex wave</t>
+  </si>
+  <si>
+    <t>Cull count will be &gt;0 but will not increase as much as the above</t>
+  </si>
+  <si>
+    <t>449.9 - 527.7</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>Manager budget increases and decreases unpredictably (using Fourier series to create random complex waves), user budget increases linearly. There are currently 10 waves that constitute this scenario</t>
+  </si>
+  <si>
+    <t>As above, but the wavelength is shorter (higher frequency) and the amplitude is smaller</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,14 +208,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -467,21 +461,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -542,9 +521,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -557,7 +535,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -576,11 +553,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,13 +567,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,7 +580,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,9 +595,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2935,10 +2911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9FB661-68A1-4497-AF3A-764ADECA08FB}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2956,415 +2932,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="26" t="s">
+      <c r="E1" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="35"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="29"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>1000</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7">
         <f>E3*50</f>
         <v>50000</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>1000</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>0</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="20">
         <f>I3*50</f>
         <v>50000</v>
       </c>
-      <c r="L3" s="27"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>1000</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>0</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11">
         <f>E4*50</f>
         <v>50000</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="12">
         <v>1000</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="12">
         <v>-3</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="21">
         <v>6325</v>
       </c>
-      <c r="L4" s="27"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>1000</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>-3</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
         <v>6325</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>1000</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>0</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="20">
         <f>I5*50</f>
         <v>50000</v>
       </c>
-      <c r="L5" s="27"/>
+      <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="24"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="32">
+        <v>1</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9">
+        <v>500</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="10">
+        <v>25000</v>
+      </c>
+      <c r="I7" s="9">
+        <v>400</v>
+      </c>
+      <c r="J7" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="K7" s="10">
+        <v>25000</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="9">
+        <v>400</v>
+      </c>
+      <c r="F8" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="10">
+        <v>25000</v>
+      </c>
+      <c r="I8" s="9">
+        <v>400</v>
+      </c>
+      <c r="J8" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="K8" s="10">
+        <v>25000</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13">
+        <v>3</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="12">
+        <v>497.7</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="10">
+        <v>25000</v>
+      </c>
+      <c r="I9" s="9">
+        <v>400</v>
+      </c>
+      <c r="J9" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="K9" s="10">
+        <v>25000</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>4</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4">
+        <v>490.73500000000001</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="10">
+        <v>25000</v>
+      </c>
+      <c r="I10" s="9">
+        <v>400</v>
+      </c>
+      <c r="J10" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="K10" s="10">
+        <v>25000</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="1">
+        <v>25000</v>
+      </c>
+      <c r="I11" s="9">
+        <v>400</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.0815999999999999</v>
+      </c>
+      <c r="K11" s="10">
+        <v>25000</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="31"/>
+      <c r="L12" s="25"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="47">
-        <v>1</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="18" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="10">
-        <v>500</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="11">
-        <v>25000</v>
-      </c>
-      <c r="I7" s="10">
-        <v>400</v>
-      </c>
-      <c r="J7" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K7" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17">
-        <v>2</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="10">
-        <v>400</v>
-      </c>
-      <c r="F8" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="G8" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="I8" s="10">
-        <v>400</v>
-      </c>
-      <c r="J8" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K8" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
-        <v>3</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="14">
-        <v>491.52100000000002</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="13">
-        <v>25000.03</v>
-      </c>
-      <c r="I9" s="10">
-        <v>400</v>
-      </c>
-      <c r="J9" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K9" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32">
-        <v>4</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5">
-        <v>490.73500000000001</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="4">
-        <v>25000.21</v>
-      </c>
-      <c r="I10" s="10">
-        <v>400</v>
-      </c>
-      <c r="J10" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K10" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="17">
-        <v>5</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="10">
-        <v>400</v>
-      </c>
-      <c r="J11" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K11" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="10">
-        <v>400</v>
-      </c>
-      <c r="J12" s="10">
-        <v>4.0815999999999999</v>
-      </c>
-      <c r="K12" s="25">
-        <v>25000.02</v>
-      </c>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>